<commit_message>
Setting up the pH sensor control board, PH4502C part_2
</commit_message>
<xml_diff>
--- a/docs/setting PH4502C.xlsx
+++ b/docs/setting PH4502C.xlsx
@@ -34,9 +34,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -64,8 +72,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -86,7 +96,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>204108</xdr:colOff>
+      <xdr:colOff>54429</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>15988</xdr:rowOff>
     </xdr:to>
@@ -441,48 +451,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A49:B52"/>
+  <dimension ref="A47:AC52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+      <selection activeCell="AN9" sqref="AN9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="49" spans="1:2">
-      <c r="A49">
+    <row r="47" spans="1:29">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+      <c r="AA47" s="1"/>
+      <c r="AB47" s="1"/>
+      <c r="AC47" s="1"/>
+    </row>
+    <row r="48" spans="1:29">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+      <c r="Y48" s="1"/>
+      <c r="Z48" s="1"/>
+      <c r="AA48" s="1"/>
+      <c r="AB48" s="1"/>
+      <c r="AC48" s="1"/>
+    </row>
+    <row r="49" spans="1:29" ht="28.5">
+      <c r="A49" s="2">
         <v>1</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+      <c r="Y49" s="1"/>
+      <c r="Z49" s="1"/>
+      <c r="AA49" s="1"/>
+      <c r="AB49" s="1"/>
+      <c r="AC49" s="1"/>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50">
+    <row r="50" spans="1:29" ht="28.5">
+      <c r="A50" s="2">
         <v>2</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
+      <c r="AC50" s="1"/>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51">
+    <row r="51" spans="1:29" ht="28.5">
+      <c r="A51" s="2">
         <v>3</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="1"/>
+      <c r="AA51" s="1"/>
+      <c r="AB51" s="1"/>
+      <c r="AC51" s="1"/>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52">
+    <row r="52" spans="1:29" ht="28.5">
+      <c r="A52" s="2">
         <v>4</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+      <c r="Y52" s="1"/>
+      <c r="Z52" s="1"/>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1"/>
+      <c r="AC52" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Setting up the pH sensor control board, PH4502C corrective
</commit_message>
<xml_diff>
--- a/docs/setting PH4502C.xlsx
+++ b/docs/setting PH4502C.xlsx
@@ -27,7 +27,7 @@
     <t>connect to J3 pins PH+ and PH-</t>
   </si>
   <si>
-    <t>Power negative GND</t>
+    <t>Power negative + Signal Ground = GND</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A47:AC52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AN9" sqref="AN9"/>
+      <selection activeCell="T51" sqref="T51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>